<commit_message>
all fleshed out, untested
</commit_message>
<xml_diff>
--- a/NCEI_test01.xlsx
+++ b/NCEI_test01.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20820" windowHeight="10060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="People &amp; Projects" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
   <si>
     <t>Can Add Multiple People</t>
   </si>
@@ -189,12 +189,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>institution</t>
-  </si>
-  <si>
-    <t>funding</t>
-  </si>
-  <si>
     <t>project</t>
   </si>
   <si>
@@ -222,9 +216,6 @@
     <t>datamethod</t>
   </si>
   <si>
-    <t>samplemethod</t>
-  </si>
-  <si>
     <t>abstract</t>
   </si>
   <si>
@@ -240,27 +231,18 @@
     <t>first2</t>
   </si>
   <si>
-    <t>middle2</t>
-  </si>
-  <si>
     <t>last2</t>
   </si>
   <si>
     <t>role2</t>
   </si>
   <si>
-    <t>email2</t>
-  </si>
-  <si>
     <t>Institution2</t>
   </si>
   <si>
     <t>funding2</t>
   </si>
   <si>
-    <t>project2</t>
-  </si>
-  <si>
     <t>ship2</t>
   </si>
   <si>
@@ -283,9 +265,6 @@
   </si>
   <si>
     <t>samplemethod2</t>
-  </si>
-  <si>
-    <t>datamethod2</t>
   </si>
   <si>
     <t>title</t>
@@ -779,7 +758,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -849,40 +828,25 @@
       <c r="E3" t="s">
         <v>54</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>55</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12">
       <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
         <v>71</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" t="s">
         <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="12"/>
@@ -1022,10 +986,10 @@
         <v>179.12344999999999</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="39" customHeight="1">
@@ -1038,10 +1002,10 @@
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="12">
@@ -1109,7 +1073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1172,48 +1136,42 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
         <v>60</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>61</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>62</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1231,7 +1189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1281,19 +1239,19 @@
     </row>
     <row r="3" spans="1:5" ht="122.25" customHeight="1">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
         <v>67</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="37" customHeight="1">

</xml_diff>

<commit_message>
filter working for all except dates
</commit_message>
<xml_diff>
--- a/NCEI_test01.xlsx
+++ b/NCEI_test01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20820" windowHeight="10060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20820" windowHeight="9880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="People &amp; Projects" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
   <si>
     <t>Can Add Multiple People</t>
   </si>
@@ -192,9 +192,6 @@
     <t>project</t>
   </si>
   <si>
-    <t>ship</t>
-  </si>
-  <si>
     <t>sea</t>
   </si>
   <si>
@@ -244,9 +241,6 @@
   </si>
   <si>
     <t>ship2</t>
-  </si>
-  <si>
-    <t>sea2</t>
   </si>
   <si>
     <t>variable2</t>
@@ -758,7 +752,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -834,19 +828,19 @@
     </row>
     <row r="4" spans="1:8" ht="12">
       <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>70</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>71</v>
-      </c>
-      <c r="G4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="12"/>
@@ -901,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -985,11 +979,8 @@
       <c r="F3">
         <v>179.12344999999999</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>56</v>
-      </c>
-      <c r="H3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="39" customHeight="1">
@@ -1002,10 +993,7 @@
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="12">
@@ -1073,7 +1061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1136,42 +1124,42 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
         <v>58</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>59</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>60</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>61</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>76</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>77</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>78</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1239,19 +1227,19 @@
     </row>
     <row r="3" spans="1:5" ht="122.25" customHeight="1">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
         <v>64</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>65</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>66</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="37" customHeight="1">

</xml_diff>